<commit_message>
Finalizando extração e alteração do work items
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vitor\Documents\UiPath\Calculate Client Security Hash\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37F6BB0F-0175-46A6-8A22-AA851450B079}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{722CDAAD-DD3E-4F78-9D33-EEE4AD2AAC83}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
   <si>
     <t>Name</t>
   </si>
@@ -146,13 +146,19 @@
   </si>
   <si>
     <t>ass_emailUser</t>
+  </si>
+  <si>
+    <t>System1_URL</t>
+  </si>
+  <si>
+    <t>https://acme-test.uipath.com/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -188,6 +194,13 @@
       <color theme="10"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -210,7 +223,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -222,6 +235,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -540,7 +554,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -646,13 +660,22 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" t="s">
+        <v>41</v>
+      </c>
+    </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="C15" s="7"/>
+    </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>

</xml_diff>